<commit_message>
Python notebook processing changes, third visualization page added to Power BI project
</commit_message>
<xml_diff>
--- a/Data/Finland_emissions_2023_main_categories.xlsx
+++ b/Data/Finland_emissions_2023_main_categories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Main category</t>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Original</t>
         </is>
       </c>
     </row>
@@ -449,6 +454,11 @@
           <t>No cat</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No cat</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -459,6 +469,11 @@
           <t>Energy</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1 Energy</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -469,6 +484,11 @@
           <t>Industrial processes and product use</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2 Industrial processes and product use</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -479,6 +499,11 @@
           <t>Agriculture</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3 Agriculture</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -489,6 +514,11 @@
           <t>Land use, land-use change and forestry (LULUCF)</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4 Land use, land-use change and forestry (LULUCF)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -497,6 +527,11 @@
       <c r="B7" t="inlineStr">
         <is>
           <t>Waste management</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5 Waste management</t>
         </is>
       </c>
     </row>

</xml_diff>